<commit_message>
OBS: Cambios generales EST: Desarrollo.
</commit_message>
<xml_diff>
--- a/registrodocentes/catalogoservicios.xlsx
+++ b/registrodocentes/catalogoservicios.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caferrerb/Dropbox/Universidad/EAM/2016-II/pa2/wk2/registrodocentes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caferrerb/git/registrodocente/registrodocentes/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="14100" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="catalogo" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Asignacion" sheetId="3" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="LISTA">Hoja2!$C$2:$C$11</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>Nombre servicio</t>
   </si>
@@ -95,13 +96,22 @@
   </si>
   <si>
     <t>Catalogo de servicios</t>
+  </si>
+  <si>
+    <t>Funcionalidad</t>
+  </si>
+  <si>
+    <t>Responsable</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -122,6 +132,19 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -166,13 +189,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D6:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,32 +503,32 @@
   </cols>
   <sheetData>
     <row r="6" spans="4:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1436,6 +1472,190 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="6">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="6">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="6">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="6">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="G9">
+        <v>6</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="6">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="G10">
+        <v>7</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="6">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="G11">
+        <v>8</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="6">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="G12">
+        <v>9</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="C13" s="4"/>
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Anexo BORegistro, RespuestaDTO y RegistroRest
</commit_message>
<xml_diff>
--- a/registrodocentes/catalogoservicios.xlsx
+++ b/registrodocentes/catalogoservicios.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caferrerb/git/registrodocente/registrodocentes/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="14100" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13290" windowHeight="5340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="catalogo" sheetId="1" r:id="rId1"/>
@@ -18,13 +13,12 @@
   </sheets>
   <definedNames>
     <definedName name="LISTA">Hoja2!$C$2:$C$11</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="METODO">Hoja2!$A$2:$A$3</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A5:G18"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -193,9 +187,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -206,6 +197,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -213,11 +207,42 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -488,31 +513,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D6:I121"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" customWidth="1"/>
-    <col min="6" max="6" width="23.83203125" customWidth="1"/>
+    <col min="4" max="4" width="24.625" customWidth="1"/>
+    <col min="5" max="5" width="12.125" customWidth="1"/>
+    <col min="6" max="6" width="23.875" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" customWidth="1"/>
-    <col min="9" max="9" width="24.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.625" customWidth="1"/>
+    <col min="9" max="9" width="24.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="4:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="D6" s="3" t="s">
+    <row r="6" spans="4:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="D6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
         <v>0</v>
       </c>
@@ -532,7 +557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -540,7 +565,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -548,7 +573,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -556,7 +581,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -564,7 +589,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -572,7 +597,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -580,7 +605,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -588,7 +613,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -596,7 +621,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -604,7 +629,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -612,7 +637,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -620,7 +645,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -628,7 +653,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -636,7 +661,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -644,7 +669,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -652,7 +677,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -660,7 +685,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -668,7 +693,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -676,7 +701,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -684,7 +709,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -692,7 +717,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -700,7 +725,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -708,7 +733,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -716,7 +741,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -724,7 +749,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -732,7 +757,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -740,7 +765,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -748,7 +773,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -756,7 +781,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -764,7 +789,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -772,7 +797,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -780,7 +805,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -788,7 +813,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -796,7 +821,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -804,7 +829,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -812,7 +837,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -820,7 +845,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -828,7 +853,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -836,7 +861,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -844,7 +869,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -852,7 +877,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -860,7 +885,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -868,7 +893,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -876,7 +901,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -884,7 +909,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -892,7 +917,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -900,7 +925,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -908,7 +933,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -916,7 +941,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -924,7 +949,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -932,7 +957,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -940,7 +965,7 @@
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -948,7 +973,7 @@
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -956,7 +981,7 @@
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -964,7 +989,7 @@
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
@@ -972,7 +997,7 @@
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
@@ -980,7 +1005,7 @@
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -988,7 +1013,7 @@
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
@@ -996,7 +1021,7 @@
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
@@ -1004,7 +1029,7 @@
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -1012,7 +1037,7 @@
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
@@ -1020,7 +1045,7 @@
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
@@ -1028,7 +1053,7 @@
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -1036,7 +1061,7 @@
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
@@ -1044,7 +1069,7 @@
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -1052,7 +1077,7 @@
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
@@ -1060,7 +1085,7 @@
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -1068,7 +1093,7 @@
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -1076,7 +1101,7 @@
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
@@ -1084,7 +1109,7 @@
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -1092,7 +1117,7 @@
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
@@ -1100,7 +1125,7 @@
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
@@ -1108,7 +1133,7 @@
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
@@ -1116,7 +1141,7 @@
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
@@ -1124,7 +1149,7 @@
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
@@ -1132,7 +1157,7 @@
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
@@ -1140,7 +1165,7 @@
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
@@ -1148,7 +1173,7 @@
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
@@ -1156,7 +1181,7 @@
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
     </row>
-    <row r="86" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
@@ -1164,7 +1189,7 @@
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
     </row>
-    <row r="87" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
@@ -1172,7 +1197,7 @@
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
     </row>
-    <row r="88" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
@@ -1180,7 +1205,7 @@
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
     </row>
-    <row r="89" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
@@ -1188,7 +1213,7 @@
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
     </row>
-    <row r="90" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
@@ -1196,7 +1221,7 @@
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
     </row>
-    <row r="91" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
@@ -1204,7 +1229,7 @@
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
     </row>
-    <row r="92" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
@@ -1212,7 +1237,7 @@
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
     </row>
-    <row r="93" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
@@ -1220,7 +1245,7 @@
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
     </row>
-    <row r="94" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
@@ -1228,7 +1253,7 @@
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
     </row>
-    <row r="95" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
@@ -1236,7 +1261,7 @@
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
     </row>
-    <row r="96" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
@@ -1244,7 +1269,7 @@
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
     </row>
-    <row r="97" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
@@ -1252,7 +1277,7 @@
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
     </row>
-    <row r="98" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
@@ -1260,7 +1285,7 @@
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
     </row>
-    <row r="99" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
@@ -1268,7 +1293,7 @@
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
     </row>
-    <row r="100" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
@@ -1276,7 +1301,7 @@
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
     </row>
-    <row r="101" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
@@ -1284,7 +1309,7 @@
       <c r="H101" s="1"/>
       <c r="I101" s="1"/>
     </row>
-    <row r="102" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
@@ -1292,7 +1317,7 @@
       <c r="H102" s="1"/>
       <c r="I102" s="1"/>
     </row>
-    <row r="103" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
@@ -1300,7 +1325,7 @@
       <c r="H103" s="1"/>
       <c r="I103" s="1"/>
     </row>
-    <row r="104" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
@@ -1308,7 +1333,7 @@
       <c r="H104" s="1"/>
       <c r="I104" s="1"/>
     </row>
-    <row r="105" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
@@ -1316,7 +1341,7 @@
       <c r="H105" s="1"/>
       <c r="I105" s="1"/>
     </row>
-    <row r="106" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
@@ -1324,7 +1349,7 @@
       <c r="H106" s="1"/>
       <c r="I106" s="1"/>
     </row>
-    <row r="107" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
@@ -1332,7 +1357,7 @@
       <c r="H107" s="1"/>
       <c r="I107" s="1"/>
     </row>
-    <row r="108" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
@@ -1340,7 +1365,7 @@
       <c r="H108" s="1"/>
       <c r="I108" s="1"/>
     </row>
-    <row r="109" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
@@ -1348,7 +1373,7 @@
       <c r="H109" s="1"/>
       <c r="I109" s="1"/>
     </row>
-    <row r="110" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="110" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
@@ -1356,7 +1381,7 @@
       <c r="H110" s="1"/>
       <c r="I110" s="1"/>
     </row>
-    <row r="111" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="111" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
@@ -1364,7 +1389,7 @@
       <c r="H111" s="1"/>
       <c r="I111" s="1"/>
     </row>
-    <row r="112" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
@@ -1372,7 +1397,7 @@
       <c r="H112" s="1"/>
       <c r="I112" s="1"/>
     </row>
-    <row r="113" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="113" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
@@ -1380,7 +1405,7 @@
       <c r="H113" s="1"/>
       <c r="I113" s="1"/>
     </row>
-    <row r="114" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
@@ -1388,7 +1413,7 @@
       <c r="H114" s="1"/>
       <c r="I114" s="1"/>
     </row>
-    <row r="115" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
@@ -1396,7 +1421,7 @@
       <c r="H115" s="1"/>
       <c r="I115" s="1"/>
     </row>
-    <row r="116" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="116" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
@@ -1404,7 +1429,7 @@
       <c r="H116" s="1"/>
       <c r="I116" s="1"/>
     </row>
-    <row r="117" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="117" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
@@ -1412,7 +1437,7 @@
       <c r="H117" s="1"/>
       <c r="I117" s="1"/>
     </row>
-    <row r="118" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="118" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
@@ -1420,7 +1445,7 @@
       <c r="H118" s="1"/>
       <c r="I118" s="1"/>
     </row>
-    <row r="119" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="119" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
@@ -1428,7 +1453,7 @@
       <c r="H119" s="1"/>
       <c r="I119" s="1"/>
     </row>
-    <row r="120" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
@@ -1436,7 +1461,7 @@
       <c r="H120" s="1"/>
       <c r="I120" s="1"/>
     </row>
-    <row r="121" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
@@ -1474,20 +1499,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -1495,8 +1520,8 @@
       </c>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="6">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="5">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1510,8 +1535,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="6">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="5">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1527,8 +1552,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="6">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="5">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1542,8 +1567,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="6">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="5">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1557,8 +1582,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="6">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="5">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1572,8 +1597,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="6">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="5">
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1587,8 +1612,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="6">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="5">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1602,8 +1627,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="6">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1617,8 +1642,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="6">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="5">
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1632,8 +1657,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="C13" s="4"/>
+    <row r="13" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="C13" s="3"/>
       <c r="G13">
         <v>10</v>
       </c>
@@ -1641,7 +1666,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
         <v>23</v>
       </c>
@@ -1662,9 +1687,9 @@
       <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1672,7 +1697,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1680,7 +1705,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1688,42 +1713,42 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Correcion servicios Rol y Acceso Cambio en la entidad Rol y Acceso (ID autoincrementable) Documentación Servicios Inserción datos en CatalogoServicios Creacion EJB RolEJB y AccesoEJB
</commit_message>
<xml_diff>
--- a/registrodocentes/catalogoservicios.xlsx
+++ b/registrodocentes/catalogoservicios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13290" windowHeight="5340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14730" windowHeight="5925" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="catalogo" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t>Nombre servicio</t>
   </si>
@@ -99,12 +99,54 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>crearRol</t>
+  </si>
+  <si>
+    <t>{
+  "obj": true,
+  "mensaje": "El Rol se registro con exito",
+  "codigo": "00"
+}</t>
+  </si>
+  <si>
+    <t>"/gestionRol/crearRol"</t>
+  </si>
+  <si>
+    <t>{
+ "rol": {
+"descripcion":"pruebaRol"
+ }
+}</t>
+  </si>
+  <si>
+    <t>"/gestionRol/listarAccesos"</t>
+  </si>
+  <si>
+    <t>listarAccesos</t>
+  </si>
+  <si>
+    <t>NADA</t>
+  </si>
+  <si>
+    <t>{
+  "obj": [
+    {
+      "id": 1,
+      "url": "UNO.HTML",
+      "nombre": "PRUEBA1"
+    }
+  ],
+  "mensaje": "Se ejecutó correctamente",
+  "codigo": "00"
+}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -183,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -202,6 +244,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -513,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D6:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -522,8 +567,8 @@
     <col min="4" max="4" width="24.625" customWidth="1"/>
     <col min="5" max="5" width="12.125" customWidth="1"/>
     <col min="6" max="6" width="23.875" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="18.625" customWidth="1"/>
+    <col min="7" max="7" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -557,21 +602,45 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+    <row r="8" spans="4:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" ht="236.25" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>

</xml_diff>

<commit_message>
Anexo serivicio de listar registros de un docente en una asignatura
</commit_message>
<xml_diff>
--- a/registrodocentes/catalogoservicios.xlsx
+++ b/registrodocentes/catalogoservicios.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
   <si>
     <t>Nombre servicio</t>
   </si>
@@ -155,12 +155,62 @@
   "codigo": "1"
 }</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>doc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Es el id del docente y </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>asig</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Es el id de la asignatura</t>
+    </r>
+  </si>
+  <si>
+    <t>/registro/listar-registros-docente-asignatura</t>
+  </si>
+  <si>
+    <t>listarRegistrosDocenteAsignatura</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -192,6 +242,14 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -571,16 +629,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D6:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="24.625" customWidth="1"/>
+    <col min="4" max="4" width="34.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.125" customWidth="1"/>
-    <col min="6" max="6" width="23.875" customWidth="1"/>
-    <col min="7" max="7" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.375" customWidth="1"/>
   </cols>
@@ -675,13 +733,25 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+    <row r="11" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
@@ -1568,6 +1638,7 @@
     <mergeCell ref="D6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">

</xml_diff>

<commit_message>
Documentacion de servicios REST y servicios añadidos a la lista de excel
</commit_message>
<xml_diff>
--- a/registrodocentes/catalogoservicios.xlsx
+++ b/registrodocentes/catalogoservicios.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\git\registrodocente\registrodocentes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12675" windowHeight="5340" tabRatio="500"/>
   </bookViews>
@@ -17,7 +22,6 @@
     <definedName name="METODO">Hoja2!$A$2:$A$3</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A9:K15"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
   <si>
     <t>Nombre servicio</t>
   </si>
@@ -205,11 +209,40 @@
   <si>
     <t>listarRegistrosDocenteAsignatura</t>
   </si>
+  <si>
+    <t>listarUsuarios</t>
+  </si>
+  <si>
+    <t>/listaUsuarios</t>
+  </si>
+  <si>
+    <t>{
+  "obj": false
+  "mensaje": "La lista esta vacia",
+  "codigo": "5"
+} else{ la lista con los usuarios }</t>
+  </si>
+  <si>
+    <t>listaCursos</t>
+  </si>
+  <si>
+    <t>/listarCursos</t>
+  </si>
+  <si>
+    <t>anio el año selecciona, periodo= 1 o 2, docente, el docente al que se le quiere ver los cursos</t>
+  </si>
+  <si>
+    <t>{
+  "obj": [],
+  "mensaje": "Proceso realizado correctamente",
+  "codigo": "00"
+}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -630,7 +663,7 @@
   <dimension ref="D6:I121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -753,21 +786,45 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+    <row r="12" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>

</xml_diff>

<commit_message>
Catalogo de servicios y cambios en controladores login y menu
</commit_message>
<xml_diff>
--- a/registrodocentes/catalogoservicios.xlsx
+++ b/registrodocentes/catalogoservicios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\git\registrodocente\registrodocentes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jairo Andres\git\registrodocente\registrodocentes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
   <si>
     <t>Nombre servicio</t>
   </si>
@@ -234,6 +234,47 @@
   <si>
     <t>{
   "obj": [],
+  "mensaje": "Proceso realizado correctamente",
+  "codigo": "00"
+}</t>
+  </si>
+  <si>
+    <t>/verificar</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>accesos</t>
+  </si>
+  <si>
+    <t>/accesos</t>
+  </si>
+  <si>
+    <t>Usuario(user) y contraseña</t>
+  </si>
+  <si>
+    <t>Usuario(user)</t>
+  </si>
+  <si>
+    <t>{
+  "obj": {
+    "accesos": [
+      {"lista de accesos"],
+    "roles": [
+      {"lista de roles y descripcion"
+  }],
+  "mensaje": "Proceso realizado correctamente",
+  "codigo": "00"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "obj": {
+    "token": "0dcb9b72-9e9c-4c40-8a31-4b3b51e62eba",
+    "usuario": "user",
+    "cedula": "1"
+  },
   "mensaje": "Proceso realizado correctamente",
   "codigo": "00"
 }</t>
@@ -662,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D6:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="E15" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -826,21 +867,45 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+    <row r="14" spans="4:9" ht="204.75" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="4:9" ht="220.5" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>

</xml_diff>

<commit_message>
servicios docentes y programas actualizados en el catalogo
</commit_message>
<xml_diff>
--- a/registrodocentes/catalogoservicios.xlsx
+++ b/registrodocentes/catalogoservicios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jairo Andres\git\registrodocente\registrodocentes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\git\registrodocente\registrodocentes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="METODO">Hoja2!$A$2:$A$3</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
   <si>
     <t>Nombre servicio</t>
   </si>
@@ -279,12 +279,88 @@
   "codigo": "00"
 }</t>
   </si>
+  <si>
+    <t>listarProgramas</t>
+  </si>
+  <si>
+    <t>/listar-programas</t>
+  </si>
+  <si>
+    <t>nada</t>
+  </si>
+  <si>
+    <t>{
+  "obj": [
+   {
+      "id": "23",
+      "nombre": "Software",
+      "facultad": {
+        "id": "1",
+        "nombre": "Ingenieria"
+      }
+    }
+  ],
+  "mensaje": "Se ejecutó correctamente",
+  "codigo": "00"
+}</t>
+  </si>
+  <si>
+    <t>listarDocentes</t>
+  </si>
+  <si>
+    <t>/listar-docentes</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>codigo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, codigo del programa</t>
+    </r>
+  </si>
+  <si>
+    <t>{
+  "obj": [
+   {
+      "id": 10000,
+      "nombre": "Triviño",
+      "apellido": "JorgeIvan",
+      "usuario": "Triviño",
+      "pass": "1234",
+      "programa": {
+        "id": "23",
+        "nombre": "Software",
+        "facultad": {
+          "id": "1",
+          "nombre": "Ingenieria"
+        }
+      }
+    }
+  ],
+  "mensaje": "Se ejecutó correctamente",
+  "codigo": "00"
+}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -324,6 +400,21 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -370,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -393,6 +484,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D6:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E15" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -857,7 +949,7 @@
       <c r="F13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="10" t="s">
         <v>43</v>
       </c>
       <c r="H13" s="7" t="s">
@@ -907,21 +999,45 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+    <row r="16" spans="4:9" ht="283.5" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>

</xml_diff>

<commit_message>
excel con los servicios de parametrizar semestre y dias no laborales
</commit_message>
<xml_diff>
--- a/registrodocentes/catalogoservicios.xlsx
+++ b/registrodocentes/catalogoservicios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\git\registrodocente\registrodocentes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JHONATAN VANEGAS\git\registrodocente\registrodocentes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="82">
   <si>
     <t>Nombre servicio</t>
   </si>
@@ -352,6 +352,89 @@
     }
   ],
   "mensaje": "Se ejecutó correctamente",
+  "codigo": "00"
+}</t>
+  </si>
+  <si>
+    <t>crearSemestre</t>
+  </si>
+  <si>
+    <t>/semestre/crearSemestre</t>
+  </si>
+  <si>
+    <t>fecha del inicio del semestre</t>
+  </si>
+  <si>
+    <t>listarSemestres</t>
+  </si>
+  <si>
+    <t>/semestre/listarSemestres</t>
+  </si>
+  <si>
+    <t>eliminarSemestre</t>
+  </si>
+  <si>
+    <t>/semestre/eliminarSemestre</t>
+  </si>
+  <si>
+    <t>año y periodo del semestre</t>
+  </si>
+  <si>
+    <t>listarDiasNoLaborales</t>
+  </si>
+  <si>
+    <t>/semestre/listarDiasNoLaborales</t>
+  </si>
+  <si>
+    <t>marcarDia</t>
+  </si>
+  <si>
+    <t>/semestre/marcarDia</t>
+  </si>
+  <si>
+    <t>DiaNoLaboralDTO, contiene el semestre, fecha del y causa del dia</t>
+  </si>
+  <si>
+    <t>eliminarDia</t>
+  </si>
+  <si>
+    <t>/semestre/eliminarDia</t>
+  </si>
+  <si>
+    <t>id del dia no laboral</t>
+  </si>
+  <si>
+    <t>{
+  "obj": true,
+ "mensaje":"semestre creo correctamente",
+  "codigo": "00"
+} else{ "error al crear" }</t>
+  </si>
+  <si>
+    <t>{
+  "obj": null,
+  "mensaje": "no hay semestres",
+  "codigo": "-1"
+} else{ la lista con lossemestres }</t>
+  </si>
+  <si>
+    <t>{
+  "obj": true,
+  "mensaje": "se elimino correctamente",
+  "codigo": "00"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "obj": null,
+  "mensaje": "no hay dias no laborales registrados",
+  "codigo": "-1"
+} else{ la lista con los dias laborales del semestre }</t>
+  </si>
+  <si>
+    <t>{
+  "obj": true,
+  "mensaje": "el dia se marco correctamente",
   "codigo": "00"
 }</t>
   </si>
@@ -478,13 +561,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D6:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:I6"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -810,14 +893,14 @@
   </cols>
   <sheetData>
     <row r="6" spans="4:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
     </row>
     <row r="7" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
@@ -949,7 +1032,7 @@
       <c r="F13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="8" t="s">
         <v>43</v>
       </c>
       <c r="H13" s="7" t="s">
@@ -1039,53 +1122,125 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+    <row r="18" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
@@ -1918,10 +2073,10 @@
       <c r="B3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="5">

</xml_diff>

<commit_message>
EJB AsignaturaDocente, SesionCurso,RegistroSesionCurso DTO AsignaturaDocente, RegistroSesionCurso Servicio rest asignaturaDocenteRest catalogo
</commit_message>
<xml_diff>
--- a/registrodocentes/catalogoservicios.xlsx
+++ b/registrodocentes/catalogoservicios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JHONATAN VANEGAS\git\registrodocente\registrodocentes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura\git\registrodocente\registrodocentes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="96">
   <si>
     <t>Nombre servicio</t>
   </si>
@@ -239,16 +239,10 @@
 }</t>
   </si>
   <si>
-    <t>/verificar</t>
-  </si>
-  <si>
     <t>login</t>
   </si>
   <si>
     <t>accesos</t>
-  </si>
-  <si>
-    <t>/accesos</t>
   </si>
   <si>
     <t>Usuario(user) y contraseña</t>
@@ -362,9 +356,6 @@
     <t>/semestre/crearSemestre</t>
   </si>
   <si>
-    <t>fecha del inicio del semestre</t>
-  </si>
-  <si>
     <t>listarSemestres</t>
   </si>
   <si>
@@ -377,9 +368,6 @@
     <t>/semestre/eliminarSemestre</t>
   </si>
   <si>
-    <t>año y periodo del semestre</t>
-  </si>
-  <si>
     <t>listarDiasNoLaborales</t>
   </si>
   <si>
@@ -392,16 +380,10 @@
     <t>/semestre/marcarDia</t>
   </si>
   <si>
-    <t>DiaNoLaboralDTO, contiene el semestre, fecha del y causa del dia</t>
-  </si>
-  <si>
     <t>eliminarDia</t>
   </si>
   <si>
     <t>/semestre/eliminarDia</t>
-  </si>
-  <si>
-    <t>id del dia no laboral</t>
   </si>
   <si>
     <t>{
@@ -436,6 +418,101 @@
   "obj": true,
   "mensaje": "el dia se marco correctamente",
   "codigo": "00"
+}</t>
+  </si>
+  <si>
+    <t>listarAsignatura</t>
+  </si>
+  <si>
+    <t>/login/verificar</t>
+  </si>
+  <si>
+    <t>/login/accesos</t>
+  </si>
+  <si>
+    <t>/asignatura/listarAsignaturas</t>
+  </si>
+  <si>
+    <t>docente</t>
+  </si>
+  <si>
+    <t>{
+  "obj": [
+    {
+      "id": "1",
+      "nombre": "Avanzada II",
+      "programa": {
+        "id": "1",
+        "nombre": "Software",
+        "facultad": {
+          "id": "1",
+          "nombre": "Ingenieria"
+        }
+      }
+    },
+    {
+      "id": "1",
+      "nombre": "Avanzada II",
+      "programa": {
+        "id": "1",
+        "nombre": "Software",
+        "facultad": {
+          "id": "1",
+          "nombre": "Ingenieria"
+        }
+      }
+    }
+  ],
+  "mensaje": "Proceso realizado correctamente",
+  "codigo": "00"
+}</t>
+  </si>
+  <si>
+    <t>tiempoSemestre</t>
+  </si>
+  <si>
+    <t>/asignatura/tiempoSemestre</t>
+  </si>
+  <si>
+    <t>AsignaturaDocenteDTO</t>
+  </si>
+  <si>
+    <t>{
+  "mensaje": "No hay horas registradas",
+  "codigo": "-1"
+}</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>DiaNoLaboralDTO,  con anho,periodo,fechaNoLaboral , causa</t>
+  </si>
+  <si>
+    <t>anho y periodo</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>tiempoMes</t>
+  </si>
+  <si>
+    <t>/asignatura//tiempoMes</t>
+  </si>
+  <si>
+    <t>RegistroSesionCursoDTO</t>
+  </si>
+  <si>
+    <t>registrosAprobados</t>
+  </si>
+  <si>
+    <t>/asignatura//registrosAprobados</t>
+  </si>
+  <si>
+    <t>{
+  "mensaje": "La asigntura no contiene registros",
+  "codigo": "-1"
 }</t>
   </si>
 </sst>
@@ -878,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D6:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1044,19 +1121,19 @@
     </row>
     <row r="14" spans="4:9" ht="204.75" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>15</v>
@@ -1064,19 +1141,19 @@
     </row>
     <row r="15" spans="4:9" ht="220.5" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="H15" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>15</v>
@@ -1084,39 +1161,39 @@
     </row>
     <row r="16" spans="4:9" ht="283.5" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>56</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="4:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>60</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
@@ -1124,19 +1201,19 @@
     </row>
     <row r="18" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="D18" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>18</v>
@@ -1144,19 +1221,19 @@
     </row>
     <row r="19" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="D19" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>18</v>
@@ -1164,19 +1241,19 @@
     </row>
     <row r="20" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="D20" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>18</v>
@@ -1184,19 +1261,19 @@
     </row>
     <row r="21" spans="4:9" ht="141.75" x14ac:dyDescent="0.25">
       <c r="D21" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>18</v>
@@ -1204,19 +1281,19 @@
     </row>
     <row r="22" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="D22" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>18</v>
@@ -1224,55 +1301,103 @@
     </row>
     <row r="23" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="D23" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
+    <row r="24" spans="4:9" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="4:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="D25" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="4:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="D26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="4:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="D27" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="28" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>

</xml_diff>

<commit_message>
Corrección de información en catalogo de servicios
</commit_message>
<xml_diff>
--- a/registrodocentes/catalogoservicios.xlsx
+++ b/registrodocentes/catalogoservicios.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura\git\registrodocente\registrodocentes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giraldo\git\registrodocente\registrodocentes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12675" windowHeight="5340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14520" windowHeight="5340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="catalogo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="99">
   <si>
     <t>Nombre servicio</t>
   </si>
@@ -151,63 +151,6 @@
   </si>
   <si>
     <t>/registro/listar-registros</t>
-  </si>
-  <si>
-    <t>{
-  "obj": [],
-  "mensaje": "Proceso realizado correctamente",
-  "codigo": "1"
-}</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>doc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, Es el id del docente y </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>asig</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, Es el id de la asignatura</t>
-    </r>
-  </si>
-  <si>
-    <t>/registro/listar-registros-docente-asignatura</t>
-  </si>
-  <si>
-    <t>listarRegistrosDocenteAsignatura</t>
   </si>
   <si>
     <t>listarUsuarios</t>
@@ -515,11 +458,36 @@
   "codigo": "-1"
 }</t>
   </si>
+  <si>
+    <t>listarRegistrosDocenteAsignaturaNA</t>
+  </si>
+  <si>
+    <t>/registro/listar-registros-docente-asignatura-sin-aprobar</t>
+  </si>
+  <si>
+    <t>aprobarRegistro</t>
+  </si>
+  <si>
+    <t>/aprobar-registro</t>
+  </si>
+  <si>
+    <t>idReg (Long)  , coment (String)</t>
+  </si>
+  <si>
+    <t>doc (int), asig (String)</t>
+  </si>
+  <si>
+    <t>{
+  "obj": "Aprobado Correctamente",
+  "mensaje": "Proceso realizado correctamente",
+  "codigo": "00"
+}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -557,14 +525,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -575,6 +535,12 @@
       <u/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -621,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -638,6 +604,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -955,29 +922,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D6:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="C27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.125" customWidth="1"/>
-    <col min="6" max="6" width="43.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="80" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="4:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
@@ -1053,7 +1020,7 @@
         <v>30</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>12</v>
@@ -1061,19 +1028,19 @@
     </row>
     <row r="11" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="D11" s="1" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>35</v>
+        <v>93</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>97</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>12</v>
@@ -1081,19 +1048,19 @@
     </row>
     <row r="12" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>14</v>
@@ -1101,19 +1068,19 @@
     </row>
     <row r="13" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>14</v>
@@ -1121,19 +1088,19 @@
     </row>
     <row r="14" spans="4:9" ht="204.75" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>15</v>
@@ -1141,19 +1108,19 @@
     </row>
     <row r="15" spans="4:9" ht="220.5" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>15</v>
@@ -1161,19 +1128,19 @@
     </row>
     <row r="16" spans="4:9" ht="283.5" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
@@ -1181,19 +1148,19 @@
     </row>
     <row r="17" spans="4:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
@@ -1201,19 +1168,19 @@
     </row>
     <row r="18" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="D18" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>18</v>
@@ -1221,19 +1188,19 @@
     </row>
     <row r="19" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="D19" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>18</v>
@@ -1241,19 +1208,19 @@
     </row>
     <row r="20" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="D20" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>18</v>
@@ -1261,19 +1228,19 @@
     </row>
     <row r="21" spans="4:9" ht="141.75" x14ac:dyDescent="0.25">
       <c r="D21" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>18</v>
@@ -1281,19 +1248,19 @@
     </row>
     <row r="22" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="D22" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>18</v>
@@ -1301,19 +1268,19 @@
     </row>
     <row r="23" spans="4:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="D23" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>18</v>
@@ -1321,19 +1288,19 @@
     </row>
     <row r="24" spans="4:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="D24" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>13</v>
@@ -1341,19 +1308,19 @@
     </row>
     <row r="25" spans="4:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="D25" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>13</v>
@@ -1361,19 +1328,19 @@
     </row>
     <row r="26" spans="4:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="D26" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>13</v>
@@ -1381,31 +1348,43 @@
     </row>
     <row r="27" spans="4:9" ht="94.5" x14ac:dyDescent="0.25">
       <c r="D27" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
+    <row r="28" spans="4:9" ht="126" x14ac:dyDescent="0.25">
+      <c r="D28" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="29" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
@@ -2198,10 +2177,10 @@
       <c r="B3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="D3" s="11"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="5">

</xml_diff>